<commit_message>
Asignación de recursos mat 8 tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="262">
   <si>
     <t>Asignatura</t>
   </si>
@@ -854,12 +854,18 @@
   <si>
     <t>Interactivo que explica los procedimientos para factorizar binomios</t>
   </si>
+  <si>
+    <t>Andrea Sabogal</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +901,14 @@
       <i/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1035,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1116,6 +1130,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,51 +1232,40 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1524,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="G2" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="H13" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1554,97 +1602,97 @@
     <col min="23" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="61" t="s">
+      <c r="Q1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="S1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="63" t="s">
+      <c r="T1" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="49"/>
+    <row r="2" spans="1:22" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="64"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="62"/>
-    </row>
-    <row r="3" spans="1:21" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="60"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="52"/>
+    </row>
+    <row r="3" spans="1:22" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1704,8 +1752,11 @@
         <f>CONCATENATE(R3,"_08_04_CO")</f>
         <v>RF_08_04_CO</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V3" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1766,58 +1817,58 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="73" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69" t="s">
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="40">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="69" t="s">
+      <c r="I5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="K5" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="70" t="s">
+      <c r="K5" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70" t="s">
+      <c r="M5" s="43"/>
+      <c r="N5" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="O5" s="69" t="s">
+      <c r="O5" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="P5" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="72">
+      <c r="P5" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="45">
         <v>6</v>
       </c>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-    </row>
-    <row r="6" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+    </row>
+    <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1872,58 +1923,58 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="73" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
+    <row r="7" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69" t="s">
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="67">
+      <c r="H7" s="40">
         <v>5</v>
       </c>
-      <c r="I7" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="69" t="s">
+      <c r="I7" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="K7" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="70" t="s">
+      <c r="K7" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M7" s="70"/>
-      <c r="N7" s="70" t="s">
+      <c r="M7" s="43"/>
+      <c r="N7" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="69" t="s">
+      <c r="O7" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P7" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="72">
+      <c r="P7" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="45">
         <v>6</v>
       </c>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="72"/>
-      <c r="U7" s="72"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1984,7 +2035,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2096,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +2157,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2167,62 +2218,62 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="67" t="s">
+    <row r="12" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69" t="s">
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="H12" s="67">
+      <c r="H12" s="40">
         <v>10</v>
       </c>
-      <c r="I12" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="69" t="s">
+      <c r="I12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="K12" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="70" t="s">
+      <c r="L12" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="73" t="s">
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="R12" s="73" t="s">
+      <c r="R12" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="S12" s="73" t="s">
+      <c r="S12" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="T12" s="73" t="s">
+      <c r="T12" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="U12" s="73" t="s">
+      <c r="U12" s="46" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2281,58 +2332,61 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:22" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="78" t="s">
         <v>243</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="79" t="s">
         <v>248</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19" t="s">
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="83">
         <v>12</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="84" t="s">
         <v>259</v>
       </c>
-      <c r="K14" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="22" t="s">
+      <c r="K14" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="18" t="s">
+      <c r="N14" s="87"/>
+      <c r="O14" s="81" t="s">
         <v>258</v>
       </c>
-      <c r="P14" s="37" t="s">
+      <c r="P14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="88">
         <v>6</v>
       </c>
-      <c r="R14" s="24"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="14"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R14" s="89"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="88"/>
+      <c r="V14" s="92" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2395,133 +2449,133 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="67" t="s">
+    <row r="16" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69" t="s">
+      <c r="F16" s="42"/>
+      <c r="G16" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="67">
+      <c r="H16" s="40">
         <v>14</v>
       </c>
-      <c r="I16" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="69" t="s">
+      <c r="I16" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="K16" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="70" t="s">
+      <c r="K16" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70" t="s">
+      <c r="M16" s="43"/>
+      <c r="N16" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="69" t="s">
+      <c r="O16" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="P16" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q16" s="72">
+      <c r="P16" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="45">
         <v>6</v>
       </c>
-      <c r="R16" s="69" t="s">
+      <c r="R16" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="S16" s="69" t="s">
+      <c r="S16" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="T16" s="72" t="str">
+      <c r="T16" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Recurso m5a-01</v>
       </c>
-      <c r="U16" s="72" t="str">
+      <c r="U16" s="45" t="str">
         <f t="shared" si="1"/>
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="67" t="s">
+    <row r="17" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69" t="s">
+      <c r="F17" s="42"/>
+      <c r="G17" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="40">
         <v>15</v>
       </c>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="69" t="s">
+      <c r="J17" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="K17" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="70" t="s">
+      <c r="K17" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="M17" s="70" t="s">
+      <c r="M17" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="N17" s="70"/>
-      <c r="O17" s="69" t="s">
+      <c r="N17" s="43"/>
+      <c r="O17" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="P17" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="72">
+      <c r="P17" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="45">
         <v>6</v>
       </c>
-      <c r="R17" s="69" t="s">
+      <c r="R17" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="S17" s="72" t="s">
+      <c r="S17" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="T17" s="72" t="str">
+      <c r="T17" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Recurso DIAP f1-01</v>
       </c>
-      <c r="U17" s="72" t="str">
+      <c r="U17" s="45" t="str">
         <f t="shared" si="1"/>
         <v>RF_08_04_CO</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2582,7 +2636,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -2643,7 +2697,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
@@ -2705,57 +2759,60 @@
         <f t="shared" si="1"/>
         <v>RF_08_04_CO</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="67" t="s">
+      <c r="V20" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69" t="s">
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="H21" s="67">
+      <c r="H21" s="40">
         <v>19</v>
       </c>
-      <c r="I21" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="69" t="s">
+      <c r="I21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="K21" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="70" t="s">
+      <c r="K21" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70" t="s">
+      <c r="M21" s="43"/>
+      <c r="N21" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="69"/>
-      <c r="P21" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q21" s="72">
+      <c r="O21" s="42"/>
+      <c r="P21" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="45">
         <v>6</v>
       </c>
-      <c r="R21" s="69"/>
-      <c r="S21" s="72"/>
-      <c r="T21" s="72"/>
-      <c r="U21" s="72"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R21" s="42"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
@@ -2816,58 +2873,61 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:22" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="78" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="79" t="s">
         <v>249</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19" t="s">
+      <c r="E23" s="80"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="83">
         <v>21</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="22" t="s">
+      <c r="K23" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="M23" s="23" t="s">
+      <c r="M23" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="N23" s="23"/>
-      <c r="O23" s="18" t="s">
+      <c r="N23" s="87"/>
+      <c r="O23" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="P23" s="37" t="s">
+      <c r="P23" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="14">
+      <c r="Q23" s="88">
         <v>6</v>
       </c>
-      <c r="R23" s="24"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="14"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R23" s="89"/>
+      <c r="S23" s="90"/>
+      <c r="T23" s="91"/>
+      <c r="U23" s="88"/>
+      <c r="V23" s="92" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
@@ -2928,70 +2988,70 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="67" t="s">
+    <row r="25" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="E25" s="69" t="s">
+      <c r="E25" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69" t="s">
+      <c r="F25" s="42"/>
+      <c r="G25" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="67">
+      <c r="H25" s="40">
         <v>23</v>
       </c>
-      <c r="I25" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="69" t="s">
+      <c r="I25" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="K25" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="70" t="s">
+      <c r="K25" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M25" s="70"/>
-      <c r="N25" s="70" t="s">
+      <c r="M25" s="43"/>
+      <c r="N25" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="O25" s="69" t="s">
+      <c r="O25" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="P25" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="72">
+      <c r="P25" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q25" s="45">
         <v>6</v>
       </c>
-      <c r="R25" s="69" t="s">
+      <c r="R25" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="S25" s="69" t="s">
+      <c r="S25" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="T25" s="72" t="str">
+      <c r="T25" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Recurso m5a-01</v>
       </c>
-      <c r="U25" s="72" t="str">
+      <c r="U25" s="45" t="str">
         <f t="shared" si="1"/>
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
@@ -3054,7 +3114,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
@@ -3105,7 +3165,7 @@
       <c r="T27" s="16"/>
       <c r="U27" s="14"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
@@ -3158,7 +3218,7 @@
       <c r="T28" s="16"/>
       <c r="U28" s="14"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -3221,7 +3281,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -3281,8 +3341,11 @@
         <f>CONCATENATE(R30,"_08_04_CO")</f>
         <v>RF_08_04_CO</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V30" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
@@ -3343,7 +3406,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>15</v>
       </c>
@@ -3404,7 +3467,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -3465,7 +3528,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -3516,7 +3579,7 @@
       <c r="T34" s="16"/>
       <c r="U34" s="14"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -3577,7 +3640,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -3640,7 +3703,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
@@ -3701,68 +3764,71 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="67" t="s">
+    <row r="38" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="67" t="s">
+      <c r="B38" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="C38" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D38" s="74" t="s">
+      <c r="D38" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69" t="s">
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="H38" s="67">
+      <c r="H38" s="40">
         <v>36</v>
       </c>
-      <c r="I38" s="67" t="s">
+      <c r="I38" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="J38" s="69" t="s">
+      <c r="J38" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="K38" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="70" t="s">
+      <c r="K38" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="M38" s="70" t="s">
+      <c r="M38" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="N38" s="70"/>
-      <c r="O38" s="69" t="s">
+      <c r="N38" s="43"/>
+      <c r="O38" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="P38" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q38" s="72">
+      <c r="P38" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="45">
         <v>6</v>
       </c>
-      <c r="R38" s="69" t="s">
+      <c r="R38" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="S38" s="72" t="s">
+      <c r="S38" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="T38" s="72" t="str">
+      <c r="T38" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Recurso f13b-01</v>
       </c>
-      <c r="U38" s="72" t="str">
+      <c r="U38" s="45" t="str">
         <f t="shared" si="1"/>
         <v>RF_08_04_CO</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V38" s="46" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -3809,7 +3875,7 @@
       <c r="T39" s="16"/>
       <c r="U39" s="14"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>15</v>
       </c>
@@ -3872,42 +3938,42 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="67" t="s">
+    <row r="41" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="67" t="s">
+      <c r="C41" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D41" s="74" t="s">
+      <c r="D41" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="69"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70" t="s">
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="O41" s="69"/>
-      <c r="P41" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q41" s="69"/>
-      <c r="R41" s="69"/>
-      <c r="S41" s="69"/>
-      <c r="T41" s="69"/>
-      <c r="U41" s="69"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O41" s="42"/>
+      <c r="P41" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="42"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
       <c r="B42" s="17"/>
       <c r="C42" s="27"/>
@@ -3930,7 +3996,7 @@
       <c r="T42" s="29"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="26"/>
       <c r="B43" s="17"/>
       <c r="C43" s="27"/>
@@ -3953,7 +4019,7 @@
       <c r="T43" s="29"/>
       <c r="U43" s="25"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="26"/>
       <c r="B44" s="17"/>
       <c r="C44" s="27"/>
@@ -3976,7 +4042,7 @@
       <c r="T44" s="29"/>
       <c r="U44" s="25"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="26"/>
       <c r="B45" s="17"/>
       <c r="C45" s="27"/>
@@ -3999,7 +4065,7 @@
       <c r="T45" s="29"/>
       <c r="U45" s="25"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="26"/>
       <c r="B46" s="17"/>
       <c r="C46" s="27"/>
@@ -4022,7 +4088,7 @@
       <c r="T46" s="29"/>
       <c r="U46" s="25"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="26"/>
       <c r="B47" s="17"/>
       <c r="C47" s="27"/>
@@ -4045,7 +4111,7 @@
       <c r="T47" s="29"/>
       <c r="U47" s="25"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="26"/>
       <c r="B48" s="17"/>
       <c r="C48" s="27"/>
@@ -4528,12 +4594,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4548,6 +4608,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">

</xml_diff>

<commit_message>
Asignación de autor recurso 35 de escaleta mat 8 tea 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -503,10 +503,6 @@
   </si>
   <si>
     <t>m102ab</t>
-  </si>
-  <si>
-    <t>se presentará inicialmente la imposibilidad de factorizar un polinómio como x^2+1 en dos factores lineales, se presentará el objeto i como número imaginario y se planteará un proyecto en le que el estudiante extenderá los casos de factorización, incluyendo suma de cubos y trinomio cuadrado imperfecto (a^2+ab+b^2) a partir de investigaciones sobre el comportamiento de los números complejos. Debe darse instrucciones precisas de qué es lo que debe consultar y cuál es el objetivo de su trabajo, para que el proceso investigativo no se vaya por caminos diferentes del de factorización. También se debe precisar el alcance de estos resultados, evitando caer en un proyecto demasiado extenso o profundo para el tema en el que está inmerso el proyecto.
-Debe centrarse el proyecto en la factorización.</t>
   </si>
   <si>
     <t>RM</t>
@@ -859,6 +855,9 @@
   </si>
   <si>
     <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Construir un F13 cons dos pestañas: Una de presentación donde se presenta un objetivo, se realiza una explicación del tema y se muestra ejemplo. Una de tarea donde se pide al estudiante poner en práctica lo expuesto en la pestaña anterior.</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1151,30 +1150,40 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1232,40 +1241,33 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1572,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="H13" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J28" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1603,94 +1605,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="71"/>
-      <c r="O1" s="59" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="88" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="66"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="52"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="89"/>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1700,7 +1702,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>123</v>
@@ -1708,7 +1710,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1717,7 +1719,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>20</v>
@@ -1730,7 +1732,7 @@
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>19</v>
@@ -1742,7 +1744,7 @@
         <v>124</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T3" s="16" t="str">
         <f>CONCATENATE("Recurso ", M3,N3,"-01")</f>
@@ -1753,7 +1755,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V3" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1764,7 +1766,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>123</v>
@@ -1781,7 +1783,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -1794,7 +1796,7 @@
         <v>22</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>19</v>
@@ -1803,10 +1805,10 @@
         <v>6</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T4" s="16" t="str">
         <f t="shared" ref="T4:T40" si="0">CONCATENATE("Recurso ", M4,N4,"-01")</f>
@@ -1825,7 +1827,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>123</v>
@@ -1833,7 +1835,7 @@
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H5" s="40">
         <v>3</v>
@@ -1842,7 +1844,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K5" s="43" t="s">
         <v>20</v>
@@ -1855,7 +1857,7 @@
         <v>119</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P5" s="44" t="s">
         <v>20</v>
@@ -1876,7 +1878,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>123</v>
@@ -1884,7 +1886,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="18"/>
       <c r="G6" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -1893,7 +1895,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>19</v>
@@ -1908,19 +1910,19 @@
         <v>19</v>
       </c>
       <c r="Q6" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="R6" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="S6" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="T6" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="T6" s="31" t="s">
+      <c r="U6" s="35" t="s">
         <v>181</v>
-      </c>
-      <c r="U6" s="35" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1931,7 +1933,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>123</v>
@@ -1939,7 +1941,7 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H7" s="40">
         <v>5</v>
@@ -1948,7 +1950,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>20</v>
@@ -1961,7 +1963,7 @@
         <v>45</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P7" s="44" t="s">
         <v>20</v>
@@ -1982,7 +1984,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>123</v>
@@ -1990,7 +1992,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -1999,7 +2001,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -2021,10 +2023,10 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2043,7 +2045,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>123</v>
@@ -2051,7 +2053,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -2060,7 +2062,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -2073,7 +2075,7 @@
         <v>33</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P9" s="37" t="s">
         <v>19</v>
@@ -2082,10 +2084,10 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S9" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T9" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2104,7 +2106,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>123</v>
@@ -2112,7 +2114,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
       <c r="G10" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -2121,7 +2123,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -2143,10 +2145,10 @@
         <v>6</v>
       </c>
       <c r="R10" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T10" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2165,7 +2167,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>123</v>
@@ -2173,7 +2175,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
@@ -2182,7 +2184,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>20</v>
@@ -2204,10 +2206,10 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S11" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T11" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2226,7 +2228,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>123</v>
@@ -2234,7 +2236,7 @@
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H12" s="40">
         <v>10</v>
@@ -2243,7 +2245,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K12" s="43" t="s">
         <v>19</v>
@@ -2258,19 +2260,19 @@
         <v>20</v>
       </c>
       <c r="Q12" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="R12" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="R12" s="46" t="s">
+      <c r="S12" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="S12" s="46" t="s">
-        <v>180</v>
-      </c>
       <c r="T12" s="46" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U12" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -2281,7 +2283,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>123</v>
@@ -2291,7 +2293,7 @@
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
@@ -2300,7 +2302,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>19</v>
@@ -2317,73 +2319,73 @@
         <v>19</v>
       </c>
       <c r="Q13" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="R13" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="R13" s="36" t="s">
+      <c r="S13" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="S13" s="35" t="s">
-        <v>180</v>
-      </c>
       <c r="T13" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U13" s="35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" s="93" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="78" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>248</v>
-      </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="82" t="s">
+      <c r="C14" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="H14" s="83">
+      <c r="H14" s="56">
         <v>12</v>
       </c>
-      <c r="I14" s="83" t="s">
+      <c r="I14" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="84" t="s">
+      <c r="J14" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="K14" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="60"/>
+      <c r="O14" s="54" t="s">
+        <v>257</v>
+      </c>
+      <c r="P14" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="61">
+        <v>6</v>
+      </c>
+      <c r="R14" s="62"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="64"/>
+      <c r="U14" s="61"/>
+      <c r="V14" s="65" t="s">
         <v>259</v>
-      </c>
-      <c r="K14" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="M14" s="87" t="s">
-        <v>56</v>
-      </c>
-      <c r="N14" s="87"/>
-      <c r="O14" s="81" t="s">
-        <v>258</v>
-      </c>
-      <c r="P14" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="88">
-        <v>6</v>
-      </c>
-      <c r="R14" s="89"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="91"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="92" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -2394,17 +2396,17 @@
         <v>122</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>132</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2413,7 +2415,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -2435,10 +2437,10 @@
         <v>6</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T15" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2457,17 +2459,17 @@
         <v>122</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>132</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H16" s="40">
         <v>14</v>
@@ -2476,7 +2478,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K16" s="43" t="s">
         <v>20</v>
@@ -2489,7 +2491,7 @@
         <v>33</v>
       </c>
       <c r="O16" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P16" s="44" t="s">
         <v>20</v>
@@ -2498,10 +2500,10 @@
         <v>6</v>
       </c>
       <c r="R16" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S16" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T16" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2520,17 +2522,17 @@
         <v>122</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>133</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="40">
         <v>15</v>
@@ -2539,7 +2541,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K17" s="43" t="s">
         <v>20</v>
@@ -2552,7 +2554,7 @@
       </c>
       <c r="N17" s="43"/>
       <c r="O17" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P17" s="44" t="s">
         <v>20</v>
@@ -2564,7 +2566,7 @@
         <v>124</v>
       </c>
       <c r="S17" s="45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T17" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2583,17 +2585,17 @@
         <v>122</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>133</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2624,7 +2626,7 @@
         <v>6</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="16" t="str">
@@ -2644,17 +2646,17 @@
         <v>122</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>134</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H19" s="8">
         <v>17</v>
@@ -2663,7 +2665,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -2685,7 +2687,7 @@
         <v>6</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="16" t="str">
@@ -2705,17 +2707,17 @@
         <v>122</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -2724,7 +2726,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -2749,7 +2751,7 @@
         <v>124</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T20" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2760,7 +2762,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V20" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
@@ -2771,15 +2773,15 @@
         <v>122</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H21" s="40">
         <v>19</v>
@@ -2788,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K21" s="43" t="s">
         <v>20</v>
@@ -2820,17 +2822,17 @@
         <v>122</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>135</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H22" s="8">
         <v>20</v>
@@ -2839,7 +2841,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -2861,7 +2863,7 @@
         <v>6</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="16" t="str">
@@ -2873,58 +2875,58 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="93" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="76" t="s">
+    <row r="23" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="78" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82" t="s">
+      <c r="C23" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" s="53"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="83">
+      <c r="H23" s="56">
         <v>21</v>
       </c>
-      <c r="I23" s="83" t="s">
+      <c r="I23" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="84" t="s">
-        <v>198</v>
-      </c>
-      <c r="K23" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="86" t="s">
+      <c r="J23" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="K23" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="M23" s="87" t="s">
+      <c r="M23" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="N23" s="87"/>
-      <c r="O23" s="81" t="s">
-        <v>254</v>
-      </c>
-      <c r="P23" s="83" t="s">
+      <c r="N23" s="60"/>
+      <c r="O23" s="54" t="s">
+        <v>253</v>
+      </c>
+      <c r="P23" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="88">
+      <c r="Q23" s="61">
         <v>6</v>
       </c>
-      <c r="R23" s="89"/>
-      <c r="S23" s="90"/>
-      <c r="T23" s="91"/>
-      <c r="U23" s="88"/>
-      <c r="V23" s="92" t="s">
-        <v>260</v>
+      <c r="R23" s="62"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="61"/>
+      <c r="V23" s="65" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -2935,17 +2937,17 @@
         <v>122</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>143</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H24" s="8">
         <v>22</v>
@@ -2954,7 +2956,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -2967,7 +2969,7 @@
         <v>25</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P24" s="37" t="s">
         <v>19</v>
@@ -2976,7 +2978,7 @@
         <v>6</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S24" s="25"/>
       <c r="T24" s="16" t="str">
@@ -2996,17 +2998,17 @@
         <v>122</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>144</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H25" s="40">
         <v>23</v>
@@ -3015,7 +3017,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>20</v>
@@ -3028,7 +3030,7 @@
         <v>33</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P25" s="44" t="s">
         <v>20</v>
@@ -3037,10 +3039,10 @@
         <v>6</v>
       </c>
       <c r="R25" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S25" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T25" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3059,17 +3061,17 @@
         <v>122</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>144</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
@@ -3078,7 +3080,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -3100,10 +3102,10 @@
         <v>6</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T26" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3122,15 +3124,15 @@
         <v>122</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H27" s="8">
         <v>25</v>
@@ -3139,7 +3141,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -3152,7 +3154,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P27" s="37" t="s">
         <v>19</v>
@@ -3173,17 +3175,17 @@
         <v>122</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H28" s="8">
         <v>26</v>
@@ -3192,7 +3194,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -3205,7 +3207,7 @@
         <v>33</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P28" s="37" t="s">
         <v>19</v>
@@ -3226,17 +3228,17 @@
         <v>122</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H29" s="8">
         <v>27</v>
@@ -3245,7 +3247,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -3267,10 +3269,10 @@
         <v>6</v>
       </c>
       <c r="R29" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S29" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T29" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3289,15 +3291,15 @@
         <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H30" s="8">
         <v>28</v>
@@ -3306,7 +3308,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -3331,7 +3333,7 @@
         <v>124</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T30" s="16" t="str">
         <f>CONCATENATE("Recurso ", M30,N30,"-01")</f>
@@ -3342,7 +3344,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V30" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -3353,15 +3355,15 @@
         <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="18"/>
       <c r="G31" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H31" s="8">
         <v>29</v>
@@ -3370,7 +3372,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
@@ -3392,10 +3394,10 @@
         <v>6</v>
       </c>
       <c r="R31" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T31" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3414,15 +3416,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="18"/>
       <c r="G32" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H32" s="8">
         <v>30</v>
@@ -3453,10 +3455,10 @@
         <v>6</v>
       </c>
       <c r="R32" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T32" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3475,10 +3477,10 @@
         <v>122</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="18"/>
@@ -3492,7 +3494,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>20</v>
@@ -3514,10 +3516,10 @@
         <v>6</v>
       </c>
       <c r="R33" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T33" s="16" t="str">
         <f t="shared" ref="T33" si="2">CONCATENATE("Recurso ", M33,N33,"-01")</f>
@@ -3536,17 +3538,17 @@
         <v>122</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H34" s="8">
         <v>32</v>
@@ -3555,7 +3557,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>20</v>
@@ -3587,10 +3589,10 @@
         <v>122</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="18"/>
@@ -3604,7 +3606,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>20</v>
@@ -3626,10 +3628,10 @@
         <v>6</v>
       </c>
       <c r="R35" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S35" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T35" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3648,17 +3650,17 @@
         <v>122</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H36" s="8">
         <v>34</v>
@@ -3667,7 +3669,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>20</v>
@@ -3689,10 +3691,10 @@
         <v>6</v>
       </c>
       <c r="R36" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T36" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3711,7 +3713,7 @@
         <v>122</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>154</v>
@@ -3719,7 +3721,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="18"/>
       <c r="G37" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H37" s="8">
         <v>35</v>
@@ -3728,7 +3730,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K37" s="21" t="s">
         <v>20</v>
@@ -3741,7 +3743,7 @@
         <v>155</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>156</v>
+        <v>261</v>
       </c>
       <c r="P37" s="37" t="s">
         <v>19</v>
@@ -3750,10 +3752,10 @@
         <v>6</v>
       </c>
       <c r="R37" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S37" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T37" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3764,7 +3766,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" s="46" customFormat="1" ht="108" x14ac:dyDescent="0.2">
       <c r="A38" s="40" t="s">
         <v>15</v>
       </c>
@@ -3772,7 +3774,7 @@
         <v>122</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D38" s="47" t="s">
         <v>154</v>
@@ -3780,16 +3782,16 @@
       <c r="E38" s="42"/>
       <c r="F38" s="42"/>
       <c r="G38" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H38" s="40">
         <v>36</v>
       </c>
       <c r="I38" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J38" s="42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K38" s="43" t="s">
         <v>20</v>
@@ -3801,8 +3803,8 @@
         <v>65</v>
       </c>
       <c r="N38" s="43"/>
-      <c r="O38" s="42" t="s">
-        <v>164</v>
+      <c r="O38" s="94" t="s">
+        <v>163</v>
       </c>
       <c r="P38" s="44" t="s">
         <v>20</v>
@@ -3814,7 +3816,7 @@
         <v>124</v>
       </c>
       <c r="S38" s="45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T38" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3825,7 +3827,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V38" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -3836,10 +3838,10 @@
         <v>122</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>10</v>
@@ -3852,10 +3854,10 @@
         <v>37</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>20</v>
@@ -3883,26 +3885,26 @@
         <v>122</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H40" s="8">
         <v>38</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>20</v>
@@ -3915,7 +3917,7 @@
         <v>33</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P40" s="37" t="s">
         <v>19</v>
@@ -3924,10 +3926,10 @@
         <v>6</v>
       </c>
       <c r="R40" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S40" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T40" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3946,10 +3948,10 @@
         <v>122</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -4594,6 +4596,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4608,12 +4616,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">

</xml_diff>

<commit_message>
Ajuste en escaleta tema 4 de mat 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
@@ -401,9 +401,6 @@
     <t>RF</t>
   </si>
   <si>
-    <t>La factorización más elemental: un monomio</t>
-  </si>
-  <si>
     <t>actividad</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
     <t>Actividad para mostrar factorizaciones de diferencia de cuadrados en las que las raices de los coeficientes no son exactas, por ejemplo: 3x^2-1=(\sqrt[3]-1)(\sqrt[3]+1)</t>
   </si>
   <si>
-    <t>Descomposición en factores de la diferencia de cuadrados con raices inexactas.</t>
-  </si>
-  <si>
     <t>Interactivo en el que se identifica la relación entre los factores de una expresión algebraica y la división algebraica</t>
   </si>
   <si>
@@ -567,15 +561,9 @@
 </t>
   </si>
   <si>
-    <t>Descubre los factores que faltan</t>
-  </si>
-  <si>
     <t>El estudiante debe arrastrar a cada contenedor los factores primos de cada monomio</t>
   </si>
   <si>
-    <t>Factorización por factor común</t>
-  </si>
-  <si>
     <t>2º ESO</t>
   </si>
   <si>
@@ -598,9 +586,6 @@
   </si>
   <si>
     <t>Halla el factor común de varios monomios</t>
-  </si>
-  <si>
-    <t>Aplicación del factor común para monomios</t>
   </si>
   <si>
     <t>Encuentra el factor común de polinomios</t>
@@ -858,6 +843,21 @@
   </si>
   <si>
     <t>Construir un F13 cons dos pestañas: Una de presentación donde se presenta un objetivo, se realiza una explicación del tema y se muestra ejemplo. Una de tarea donde se pide al estudiante poner en práctica lo expuesto en la pestaña anterior.</t>
+  </si>
+  <si>
+    <t>Factoriza monomios</t>
+  </si>
+  <si>
+    <t>Descompone monomios en factores</t>
+  </si>
+  <si>
+    <t>Factoriza encontrando el factor común</t>
+  </si>
+  <si>
+    <t>Aplicac el factor común para monomios</t>
+  </si>
+  <si>
+    <t>Factoriza diferencia de cuadrados con raíces inexactas</t>
   </si>
 </sst>
 </file>
@@ -1184,6 +1184,33 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1240,33 +1267,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1574,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J28" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1605,94 +1605,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="M1" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="81"/>
-      <c r="O1" s="69" t="s">
+      <c r="N1" s="90"/>
+      <c r="O1" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="86" t="s">
+      <c r="P1" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="88" t="s">
+      <c r="Q1" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="92" t="s">
+      <c r="R1" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="88" t="s">
+      <c r="S1" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="90" t="s">
+      <c r="T1" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="88" t="s">
+      <c r="U1" s="70" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="89"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1702,7 +1702,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>123</v>
@@ -1710,7 +1710,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1719,7 +1719,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>20</v>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>19</v>
@@ -1744,7 +1744,7 @@
         <v>124</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T3" s="16" t="str">
         <f>CONCATENATE("Recurso ", M3,N3,"-01")</f>
@@ -1755,7 +1755,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V3" s="30" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1766,7 +1766,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>123</v>
@@ -1774,7 +1774,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>125</v>
+        <v>257</v>
       </c>
       <c r="H4" s="8">
         <v>2</v>
@@ -1783,20 +1783,20 @@
         <v>20</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M4" s="23"/>
       <c r="N4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>19</v>
@@ -1805,10 +1805,10 @@
         <v>6</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T4" s="16" t="str">
         <f t="shared" ref="T4:T40" si="0">CONCATENATE("Recurso ", M4,N4,"-01")</f>
@@ -1827,7 +1827,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>123</v>
@@ -1835,7 +1835,7 @@
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42" t="s">
-        <v>174</v>
+        <v>258</v>
       </c>
       <c r="H5" s="40">
         <v>3</v>
@@ -1844,20 +1844,20 @@
         <v>20</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="K5" s="43" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="43"/>
       <c r="N5" s="43" t="s">
         <v>119</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P5" s="44" t="s">
         <v>20</v>
@@ -1878,7 +1878,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>123</v>
@@ -1886,7 +1886,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="18"/>
       <c r="G6" s="19" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -1895,13 +1895,13 @@
         <v>20</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
@@ -1910,19 +1910,19 @@
         <v>19</v>
       </c>
       <c r="Q6" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="R6" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="T6" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="U6" s="35" t="s">
         <v>177</v>
-      </c>
-      <c r="R6" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="T6" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="U6" s="35" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>123</v>
@@ -1941,7 +1941,7 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H7" s="40">
         <v>5</v>
@@ -1950,20 +1950,20 @@
         <v>20</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M7" s="43"/>
       <c r="N7" s="43" t="s">
         <v>45</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P7" s="44" t="s">
         <v>20</v>
@@ -1984,7 +1984,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>123</v>
@@ -1992,7 +1992,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -2001,20 +2001,20 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M8" s="23"/>
       <c r="N8" s="23" t="s">
         <v>27</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P8" s="37" t="s">
         <v>19</v>
@@ -2023,10 +2023,10 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2045,7 +2045,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>123</v>
@@ -2053,7 +2053,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19" t="s">
-        <v>185</v>
+        <v>260</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -2062,20 +2062,20 @@
         <v>20</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M9" s="23"/>
       <c r="N9" s="23" t="s">
         <v>33</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="P9" s="37" t="s">
         <v>19</v>
@@ -2084,10 +2084,10 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S9" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T9" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2106,7 +2106,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>123</v>
@@ -2114,7 +2114,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
       <c r="G10" s="19" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -2123,20 +2123,20 @@
         <v>20</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M10" s="23"/>
       <c r="N10" s="23" t="s">
         <v>22</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P10" s="37" t="s">
         <v>19</v>
@@ -2145,10 +2145,10 @@
         <v>6</v>
       </c>
       <c r="R10" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T10" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2167,7 +2167,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>123</v>
@@ -2175,7 +2175,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
@@ -2184,20 +2184,20 @@
         <v>20</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23" t="s">
         <v>27</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P11" s="37" t="s">
         <v>19</v>
@@ -2206,10 +2206,10 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S11" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T11" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2228,7 +2228,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>123</v>
@@ -2236,7 +2236,7 @@
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H12" s="40">
         <v>10</v>
@@ -2245,13 +2245,13 @@
         <v>20</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K12" s="43" t="s">
         <v>19</v>
       </c>
       <c r="L12" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
@@ -2260,19 +2260,19 @@
         <v>20</v>
       </c>
       <c r="Q12" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="R12" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="S12" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="T12" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="U12" s="46" t="s">
         <v>177</v>
-      </c>
-      <c r="R12" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="S12" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="T12" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="U12" s="46" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -2283,17 +2283,17 @@
         <v>122</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>123</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="19" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
@@ -2302,13 +2302,13 @@
         <v>20</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>19</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M13" s="23"/>
       <c r="N13" s="23" t="s">
@@ -2319,19 +2319,19 @@
         <v>19</v>
       </c>
       <c r="Q13" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="R13" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="S13" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="T13" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="U13" s="35" t="s">
         <v>177</v>
-      </c>
-      <c r="R13" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="S13" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="T13" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="U13" s="35" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -2342,15 +2342,15 @@
         <v>122</v>
       </c>
       <c r="C14" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="52" t="s">
         <v>242</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>247</v>
       </c>
       <c r="E14" s="53"/>
       <c r="F14" s="54"/>
       <c r="G14" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14" s="56">
         <v>12</v>
@@ -2359,7 +2359,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="57" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K14" s="58" t="s">
         <v>20</v>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="N14" s="60"/>
       <c r="O14" s="54" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P14" s="56" t="s">
         <v>19</v>
@@ -2385,7 +2385,7 @@
       <c r="T14" s="64"/>
       <c r="U14" s="61"/>
       <c r="V14" s="65" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -2396,17 +2396,17 @@
         <v>122</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>247</v>
-      </c>
       <c r="E15" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2415,20 +2415,20 @@
         <v>20</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M15" s="23"/>
       <c r="N15" s="23" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P15" s="37" t="s">
         <v>19</v>
@@ -2437,10 +2437,10 @@
         <v>6</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T15" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2459,17 +2459,17 @@
         <v>122</v>
       </c>
       <c r="C16" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="D16" s="41" t="s">
-        <v>247</v>
-      </c>
       <c r="E16" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42" t="s">
-        <v>160</v>
+        <v>261</v>
       </c>
       <c r="H16" s="40">
         <v>14</v>
@@ -2478,20 +2478,20 @@
         <v>20</v>
       </c>
       <c r="J16" s="42" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K16" s="43" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M16" s="43"/>
       <c r="N16" s="43" t="s">
         <v>33</v>
       </c>
       <c r="O16" s="42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P16" s="44" t="s">
         <v>20</v>
@@ -2500,10 +2500,10 @@
         <v>6</v>
       </c>
       <c r="R16" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S16" s="42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T16" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2514,7 +2514,7 @@
         <v>RM_08_04_CO</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" s="46" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
         <v>15</v>
       </c>
@@ -2522,17 +2522,17 @@
         <v>122</v>
       </c>
       <c r="C17" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D17" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="D17" s="41" t="s">
-        <v>247</v>
-      </c>
       <c r="E17" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H17" s="40">
         <v>15</v>
@@ -2541,7 +2541,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K17" s="43" t="s">
         <v>20</v>
@@ -2553,8 +2553,8 @@
         <v>118</v>
       </c>
       <c r="N17" s="43"/>
-      <c r="O17" s="42" t="s">
-        <v>167</v>
+      <c r="O17" s="67" t="s">
+        <v>165</v>
       </c>
       <c r="P17" s="44" t="s">
         <v>20</v>
@@ -2566,7 +2566,7 @@
         <v>124</v>
       </c>
       <c r="S17" s="45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T17" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2585,17 +2585,17 @@
         <v>122</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>247</v>
-      </c>
       <c r="E18" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="19" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2604,20 +2604,20 @@
         <v>20</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M18" s="23"/>
       <c r="N18" s="23" t="s">
         <v>22</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P18" s="37" t="s">
         <v>19</v>
@@ -2626,7 +2626,7 @@
         <v>6</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="16" t="str">
@@ -2646,17 +2646,17 @@
         <v>122</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>247</v>
-      </c>
       <c r="E19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="19" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H19" s="8">
         <v>17</v>
@@ -2665,20 +2665,20 @@
         <v>20</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M19" s="23"/>
       <c r="N19" s="23" t="s">
         <v>39</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P19" s="37" t="s">
         <v>19</v>
@@ -2687,7 +2687,7 @@
         <v>6</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="16" t="str">
@@ -2707,17 +2707,17 @@
         <v>122</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="D20" s="32" t="s">
-        <v>247</v>
-      </c>
       <c r="E20" s="17" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="19" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -2726,7 +2726,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="N20" s="23"/>
       <c r="O20" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P20" s="37" t="s">
         <v>19</v>
@@ -2751,7 +2751,7 @@
         <v>124</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T20" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2762,7 +2762,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V20" s="30" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
@@ -2773,15 +2773,15 @@
         <v>122</v>
       </c>
       <c r="C21" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="41" t="s">
         <v>242</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>247</v>
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H21" s="40">
         <v>19</v>
@@ -2790,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K21" s="43" t="s">
         <v>20</v>
@@ -2822,17 +2822,17 @@
         <v>122</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="D22" s="32" t="s">
-        <v>247</v>
-      </c>
       <c r="E22" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H22" s="8">
         <v>20</v>
@@ -2841,20 +2841,20 @@
         <v>20</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M22" s="23"/>
       <c r="N22" s="23" t="s">
         <v>52</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P22" s="37" t="s">
         <v>19</v>
@@ -2863,7 +2863,7 @@
         <v>6</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="16" t="str">
@@ -2883,15 +2883,15 @@
         <v>122</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="54"/>
       <c r="G23" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H23" s="56">
         <v>21</v>
@@ -2900,7 +2900,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K23" s="58" t="s">
         <v>20</v>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="N23" s="60"/>
       <c r="O23" s="54" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="P23" s="56" t="s">
         <v>19</v>
@@ -2926,7 +2926,7 @@
       <c r="T23" s="64"/>
       <c r="U23" s="61"/>
       <c r="V23" s="65" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -2937,17 +2937,17 @@
         <v>122</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="19" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H24" s="8">
         <v>22</v>
@@ -2956,20 +2956,20 @@
         <v>20</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M24" s="23"/>
       <c r="N24" s="23" t="s">
         <v>25</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="P24" s="37" t="s">
         <v>19</v>
@@ -2978,7 +2978,7 @@
         <v>6</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S24" s="25"/>
       <c r="T24" s="16" t="str">
@@ -2998,17 +2998,17 @@
         <v>122</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H25" s="40">
         <v>23</v>
@@ -3017,20 +3017,20 @@
         <v>20</v>
       </c>
       <c r="J25" s="42" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M25" s="43"/>
       <c r="N25" s="43" t="s">
         <v>33</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P25" s="44" t="s">
         <v>20</v>
@@ -3039,10 +3039,10 @@
         <v>6</v>
       </c>
       <c r="R25" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S25" s="42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T25" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3061,17 +3061,17 @@
         <v>122</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="19" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
@@ -3080,20 +3080,20 @@
         <v>20</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M26" s="23"/>
       <c r="N26" s="23" t="s">
         <v>29</v>
       </c>
       <c r="O26" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P26" s="37" t="s">
         <v>19</v>
@@ -3102,10 +3102,10 @@
         <v>6</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T26" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3124,15 +3124,15 @@
         <v>122</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H27" s="8">
         <v>25</v>
@@ -3141,7 +3141,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -3154,7 +3154,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="P27" s="37" t="s">
         <v>19</v>
@@ -3175,17 +3175,17 @@
         <v>122</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H28" s="8">
         <v>26</v>
@@ -3194,7 +3194,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -3207,7 +3207,7 @@
         <v>33</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="P28" s="37" t="s">
         <v>19</v>
@@ -3228,17 +3228,17 @@
         <v>122</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H29" s="8">
         <v>27</v>
@@ -3247,20 +3247,20 @@
         <v>20</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M29" s="23"/>
       <c r="N29" s="23" t="s">
         <v>52</v>
       </c>
       <c r="O29" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P29" s="37" t="s">
         <v>19</v>
@@ -3269,10 +3269,10 @@
         <v>6</v>
       </c>
       <c r="R29" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S29" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T29" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3291,15 +3291,15 @@
         <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="19" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H30" s="8">
         <v>28</v>
@@ -3308,7 +3308,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="N30" s="23"/>
       <c r="O30" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P30" s="37" t="s">
         <v>19</v>
@@ -3333,7 +3333,7 @@
         <v>124</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T30" s="16" t="str">
         <f>CONCATENATE("Recurso ", M30,N30,"-01")</f>
@@ -3344,7 +3344,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V30" s="30" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -3355,15 +3355,15 @@
         <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="18"/>
       <c r="G31" s="19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H31" s="8">
         <v>29</v>
@@ -3372,20 +3372,20 @@
         <v>20</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M31" s="23"/>
       <c r="N31" s="23" t="s">
         <v>29</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P31" s="37" t="s">
         <v>19</v>
@@ -3394,10 +3394,10 @@
         <v>6</v>
       </c>
       <c r="R31" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T31" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3416,15 +3416,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="18"/>
       <c r="G32" s="19" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H32" s="8">
         <v>30</v>
@@ -3433,20 +3433,20 @@
         <v>20</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K32" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M32" s="23"/>
       <c r="N32" s="23" t="s">
         <v>33</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P32" s="37" t="s">
         <v>19</v>
@@ -3455,10 +3455,10 @@
         <v>6</v>
       </c>
       <c r="R32" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T32" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3477,15 +3477,15 @@
         <v>122</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="18"/>
       <c r="G33" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H33" s="8">
         <v>31</v>
@@ -3494,20 +3494,20 @@
         <v>20</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M33" s="23"/>
       <c r="N33" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O33" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P33" s="37" t="s">
         <v>19</v>
@@ -3516,10 +3516,10 @@
         <v>6</v>
       </c>
       <c r="R33" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T33" s="16" t="str">
         <f t="shared" ref="T33" si="2">CONCATENATE("Recurso ", M33,N33,"-01")</f>
@@ -3538,17 +3538,17 @@
         <v>122</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="19" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H34" s="8">
         <v>32</v>
@@ -3557,7 +3557,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>20</v>
@@ -3589,15 +3589,15 @@
         <v>122</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="18"/>
       <c r="G35" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H35" s="8">
         <v>33</v>
@@ -3606,20 +3606,20 @@
         <v>20</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M35" s="23"/>
       <c r="N35" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P35" s="37" t="s">
         <v>19</v>
@@ -3628,10 +3628,10 @@
         <v>6</v>
       </c>
       <c r="R35" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S35" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T35" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3650,17 +3650,17 @@
         <v>122</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="19" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H36" s="8">
         <v>34</v>
@@ -3669,20 +3669,20 @@
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M36" s="23"/>
       <c r="N36" s="23" t="s">
         <v>52</v>
       </c>
       <c r="O36" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P36" s="37" t="s">
         <v>19</v>
@@ -3691,10 +3691,10 @@
         <v>6</v>
       </c>
       <c r="R36" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T36" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3713,15 +3713,15 @@
         <v>122</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="18"/>
       <c r="G37" s="19" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H37" s="8">
         <v>35</v>
@@ -3730,20 +3730,20 @@
         <v>20</v>
       </c>
       <c r="J37" s="20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="K37" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M37" s="23"/>
       <c r="N37" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="P37" s="37" t="s">
         <v>19</v>
@@ -3752,10 +3752,10 @@
         <v>6</v>
       </c>
       <c r="R37" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S37" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T37" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3774,24 +3774,24 @@
         <v>122</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="42"/>
       <c r="F38" s="42"/>
       <c r="G38" s="42" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H38" s="40">
         <v>36</v>
       </c>
       <c r="I38" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J38" s="42" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K38" s="43" t="s">
         <v>20</v>
@@ -3803,8 +3803,8 @@
         <v>65</v>
       </c>
       <c r="N38" s="43"/>
-      <c r="O38" s="94" t="s">
-        <v>163</v>
+      <c r="O38" s="67" t="s">
+        <v>161</v>
       </c>
       <c r="P38" s="44" t="s">
         <v>20</v>
@@ -3816,7 +3816,7 @@
         <v>124</v>
       </c>
       <c r="S38" s="45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T38" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3827,7 +3827,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V38" s="46" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -3838,10 +3838,10 @@
         <v>122</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>10</v>
@@ -3854,10 +3854,10 @@
         <v>37</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>20</v>
@@ -3885,39 +3885,39 @@
         <v>122</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H40" s="8">
         <v>38</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M40" s="23"/>
       <c r="N40" s="23" t="s">
         <v>33</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P40" s="37" t="s">
         <v>19</v>
@@ -3926,10 +3926,10 @@
         <v>6</v>
       </c>
       <c r="R40" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S40" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T40" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3948,10 +3948,10 @@
         <v>122</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -4596,12 +4596,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4616,6 +4610,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">

</xml_diff>

<commit_message>
Ajuste de recursos en escaleta mat 8 tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/Escaleta MA_08_04_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="263">
   <si>
     <t>Asignatura</t>
   </si>
@@ -525,9 +525,6 @@
 Se puede proponer la lectura del Diablo de los número en el apartado que trabaja este tema.</t>
   </si>
   <si>
-    <t>División y factorización de trinomios</t>
-  </si>
-  <si>
     <t>Incluir ejemplos de divisiones de trinomios y binomios, de tal forma que el estudiante identifique la relación entre ser factor de un trinomio y una división exacta. Se debe resaltar, con ejercicios, el hecho que si al hacer una división no es exacta, el divisor no puede ser un factor de la descomposición factorial del polinomio que está en el dividendo.</t>
   </si>
   <si>
@@ -624,21 +621,12 @@
     <t>interactivo en el que se explica cómo se factorizan trinomios según su clasificación</t>
   </si>
   <si>
-    <t>Trinomios de la forma x2n + bxn + c</t>
-  </si>
-  <si>
-    <t>Aplicaciones de la factorización de binomios</t>
-  </si>
-  <si>
     <t>Actividades de cálculo de áreas, perímetro, capcaidad etc aplicandola factorización</t>
   </si>
   <si>
     <t>Recurso en el que se propondrán trinomios de la forma x2n + bxn + c que deben ser factorizados y el estudiante deberá la factorización correcta. Se deben proponer en orden de dificultad creciente.</t>
   </si>
   <si>
-    <t>Trinomios de la forma ax2n + bxn + c</t>
-  </si>
-  <si>
     <t>Factorización de cubos perfectos</t>
   </si>
   <si>
@@ -664,12 +652,6 @@
   </si>
   <si>
     <t>Actividad sobre La factorización completa</t>
-  </si>
-  <si>
-    <t>Problemas de aplicación</t>
-  </si>
-  <si>
-    <t>Expresiones ocultas</t>
   </si>
   <si>
     <t>En la izquierda aparecen expresiones como __ + 11a + __ = (2a + 1)(5a + 3) y a la derecha las opciones que pueden completar la expresión</t>
@@ -858,6 +840,27 @@
   </si>
   <si>
     <t>Factoriza diferencia de cuadrados con raíces inexactas</t>
+  </si>
+  <si>
+    <t>Aplica la factorización de binomios</t>
+  </si>
+  <si>
+    <t>Trabaja con trinomios de la forma x²ⁿ + bxⁿ + c</t>
+  </si>
+  <si>
+    <t>Relaciona la división y la factorización de trinomios</t>
+  </si>
+  <si>
+    <t>Factoriza trinomios de la forma ax2n + bnx + c</t>
+  </si>
+  <si>
+    <t>Encuentra las expresiones ocultas</t>
+  </si>
+  <si>
+    <t>Resuelve problemas aplicando la factorización</t>
+  </si>
+  <si>
+    <t>Factoriza polinomios aplicando varios casos</t>
   </si>
 </sst>
 </file>
@@ -1187,30 +1190,6 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,6 +1245,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1574,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D10" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1605,94 +1608,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="76" t="s">
+      <c r="H1" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="84" t="s">
+      <c r="L1" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="90" t="s">
+      <c r="M1" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="90"/>
-      <c r="O1" s="78" t="s">
+      <c r="N1" s="82"/>
+      <c r="O1" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="68" t="s">
+      <c r="P1" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="74" t="s">
+      <c r="R1" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="70" t="s">
+      <c r="S1" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="72" t="s">
+      <c r="T1" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="70" t="s">
+      <c r="U1" s="89" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="85"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="77"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="90"/>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1702,7 +1705,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>123</v>
@@ -1710,7 +1713,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1719,7 +1722,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>20</v>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>19</v>
@@ -1744,7 +1747,7 @@
         <v>124</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T3" s="16" t="str">
         <f>CONCATENATE("Recurso ", M3,N3,"-01")</f>
@@ -1755,7 +1758,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V3" s="30" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1766,7 +1769,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>123</v>
@@ -1774,7 +1777,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H4" s="8">
         <v>2</v>
@@ -1783,7 +1786,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -1796,7 +1799,7 @@
         <v>22</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>19</v>
@@ -1808,7 +1811,7 @@
         <v>155</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T4" s="16" t="str">
         <f t="shared" ref="T4:T40" si="0">CONCATENATE("Recurso ", M4,N4,"-01")</f>
@@ -1827,7 +1830,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>123</v>
@@ -1835,7 +1838,7 @@
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="H5" s="40">
         <v>3</v>
@@ -1844,7 +1847,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="K5" s="43" t="s">
         <v>20</v>
@@ -1857,7 +1860,7 @@
         <v>119</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P5" s="44" t="s">
         <v>20</v>
@@ -1878,7 +1881,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>123</v>
@@ -1886,7 +1889,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="18"/>
       <c r="G6" s="19" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -1895,7 +1898,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>19</v>
@@ -1910,19 +1913,19 @@
         <v>19</v>
       </c>
       <c r="Q6" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="R6" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="S6" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="T6" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="T6" s="31" t="s">
+      <c r="U6" s="35" t="s">
         <v>176</v>
-      </c>
-      <c r="U6" s="35" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1933,7 +1936,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>123</v>
@@ -1941,7 +1944,7 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H7" s="40">
         <v>5</v>
@@ -1950,7 +1953,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>20</v>
@@ -1963,7 +1966,7 @@
         <v>45</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P7" s="44" t="s">
         <v>20</v>
@@ -1984,7 +1987,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>123</v>
@@ -1992,7 +1995,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -2001,7 +2004,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -2026,7 +2029,7 @@
         <v>155</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2045,7 +2048,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>123</v>
@@ -2053,7 +2056,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -2062,7 +2065,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -2075,7 +2078,7 @@
         <v>33</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="P9" s="37" t="s">
         <v>19</v>
@@ -2087,7 +2090,7 @@
         <v>155</v>
       </c>
       <c r="S9" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T9" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2106,7 +2109,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>123</v>
@@ -2114,7 +2117,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
       <c r="G10" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -2123,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -2148,7 +2151,7 @@
         <v>155</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T10" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2167,7 +2170,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>123</v>
@@ -2175,7 +2178,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
@@ -2184,7 +2187,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>20</v>
@@ -2209,7 +2212,7 @@
         <v>155</v>
       </c>
       <c r="S11" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T11" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2228,7 +2231,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>123</v>
@@ -2236,7 +2239,7 @@
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H12" s="40">
         <v>10</v>
@@ -2245,7 +2248,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="K12" s="43" t="s">
         <v>19</v>
@@ -2260,19 +2263,19 @@
         <v>20</v>
       </c>
       <c r="Q12" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="R12" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="R12" s="46" t="s">
+      <c r="S12" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="S12" s="46" t="s">
-        <v>175</v>
-      </c>
       <c r="T12" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U12" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -2283,7 +2286,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>123</v>
@@ -2293,7 +2296,7 @@
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="19" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
@@ -2302,7 +2305,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>19</v>
@@ -2319,19 +2322,19 @@
         <v>19</v>
       </c>
       <c r="Q13" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="R13" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="R13" s="36" t="s">
+      <c r="S13" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="S13" s="35" t="s">
-        <v>175</v>
-      </c>
       <c r="T13" s="31" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="U13" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -2342,10 +2345,10 @@
         <v>122</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D14" s="52" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E14" s="53"/>
       <c r="F14" s="54"/>
@@ -2359,7 +2362,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="57" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K14" s="58" t="s">
         <v>20</v>
@@ -2372,7 +2375,7 @@
       </c>
       <c r="N14" s="60"/>
       <c r="O14" s="54" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="P14" s="56" t="s">
         <v>19</v>
@@ -2385,7 +2388,7 @@
       <c r="T14" s="64"/>
       <c r="U14" s="61"/>
       <c r="V14" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -2396,17 +2399,17 @@
         <v>122</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>131</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2415,7 +2418,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -2440,7 +2443,7 @@
         <v>155</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T15" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2459,17 +2462,17 @@
         <v>122</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>131</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H16" s="40">
         <v>14</v>
@@ -2478,7 +2481,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="42" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K16" s="43" t="s">
         <v>20</v>
@@ -2503,7 +2506,7 @@
         <v>155</v>
       </c>
       <c r="S16" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T16" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2522,17 +2525,17 @@
         <v>122</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>132</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H17" s="40">
         <v>15</v>
@@ -2554,7 +2557,7 @@
       </c>
       <c r="N17" s="43"/>
       <c r="O17" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P17" s="44" t="s">
         <v>20</v>
@@ -2566,7 +2569,7 @@
         <v>124</v>
       </c>
       <c r="S17" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T17" s="45" t="str">
         <f t="shared" si="0"/>
@@ -2585,17 +2588,17 @@
         <v>122</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>132</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2646,17 +2649,17 @@
         <v>122</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>133</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H19" s="8">
         <v>17</v>
@@ -2665,7 +2668,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -2707,17 +2710,17 @@
         <v>122</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -2726,7 +2729,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -2751,7 +2754,7 @@
         <v>124</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T20" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2762,7 +2765,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V20" s="30" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="46" customFormat="1" x14ac:dyDescent="0.2">
@@ -2773,15 +2776,15 @@
         <v>122</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42" t="s">
-        <v>194</v>
+        <v>256</v>
       </c>
       <c r="H21" s="40">
         <v>19</v>
@@ -2790,7 +2793,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K21" s="43" t="s">
         <v>20</v>
@@ -2822,17 +2825,17 @@
         <v>122</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>134</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H22" s="8">
         <v>20</v>
@@ -2841,7 +2844,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -2883,10 +2886,10 @@
         <v>122</v>
       </c>
       <c r="C23" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="52" t="s">
         <v>237</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>243</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="54"/>
@@ -2900,7 +2903,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K23" s="58" t="s">
         <v>20</v>
@@ -2913,7 +2916,7 @@
       </c>
       <c r="N23" s="60"/>
       <c r="O23" s="54" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="P23" s="56" t="s">
         <v>19</v>
@@ -2926,7 +2929,7 @@
       <c r="T23" s="64"/>
       <c r="U23" s="61"/>
       <c r="V23" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -2937,17 +2940,17 @@
         <v>122</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>142</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="19" t="s">
-        <v>193</v>
+        <v>257</v>
       </c>
       <c r="H24" s="8">
         <v>22</v>
@@ -2956,7 +2959,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -2969,7 +2972,7 @@
         <v>25</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="P24" s="37" t="s">
         <v>19</v>
@@ -2998,17 +3001,17 @@
         <v>122</v>
       </c>
       <c r="C25" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" s="41" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>243</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>143</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42" t="s">
-        <v>162</v>
+        <v>258</v>
       </c>
       <c r="H25" s="40">
         <v>23</v>
@@ -3017,7 +3020,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="42" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>20</v>
@@ -3030,7 +3033,7 @@
         <v>33</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P25" s="44" t="s">
         <v>20</v>
@@ -3042,7 +3045,7 @@
         <v>155</v>
       </c>
       <c r="S25" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T25" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3061,17 +3064,17 @@
         <v>122</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>143</v>
       </c>
       <c r="F26" s="18"/>
-      <c r="G26" s="19" t="s">
-        <v>197</v>
+      <c r="G26" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
@@ -3080,7 +3083,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -3105,7 +3108,7 @@
         <v>155</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T26" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3124,15 +3127,15 @@
         <v>122</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="H27" s="8">
         <v>25</v>
@@ -3141,7 +3144,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -3154,7 +3157,7 @@
         <v>39</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="P27" s="37" t="s">
         <v>19</v>
@@ -3175,17 +3178,17 @@
         <v>122</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="19" t="s">
-        <v>207</v>
+        <v>261</v>
       </c>
       <c r="H28" s="8">
         <v>26</v>
@@ -3194,7 +3197,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -3207,7 +3210,7 @@
         <v>33</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="P28" s="37" t="s">
         <v>19</v>
@@ -3228,17 +3231,17 @@
         <v>122</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H29" s="8">
         <v>27</v>
@@ -3247,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -3272,7 +3275,7 @@
         <v>155</v>
       </c>
       <c r="S29" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T29" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3291,15 +3294,15 @@
         <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H30" s="8">
         <v>28</v>
@@ -3308,7 +3311,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -3333,7 +3336,7 @@
         <v>124</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T30" s="16" t="str">
         <f>CONCATENATE("Recurso ", M30,N30,"-01")</f>
@@ -3344,7 +3347,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V30" s="30" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -3355,15 +3358,15 @@
         <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="18"/>
       <c r="G31" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H31" s="8">
         <v>29</v>
@@ -3372,7 +3375,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>20</v>
@@ -3397,7 +3400,7 @@
         <v>155</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T31" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3416,15 +3419,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="18"/>
       <c r="G32" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H32" s="8">
         <v>30</v>
@@ -3458,7 +3461,7 @@
         <v>155</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T32" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3477,15 +3480,15 @@
         <v>122</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="18"/>
       <c r="G33" s="19" t="s">
-        <v>150</v>
+        <v>262</v>
       </c>
       <c r="H33" s="8">
         <v>31</v>
@@ -3494,7 +3497,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>20</v>
@@ -3519,7 +3522,7 @@
         <v>155</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T33" s="16" t="str">
         <f t="shared" ref="T33" si="2">CONCATENATE("Recurso ", M33,N33,"-01")</f>
@@ -3538,17 +3541,17 @@
         <v>122</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="19" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H34" s="8">
         <v>32</v>
@@ -3557,7 +3560,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>20</v>
@@ -3589,10 +3592,10 @@
         <v>122</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="18"/>
@@ -3606,7 +3609,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>20</v>
@@ -3631,7 +3634,7 @@
         <v>155</v>
       </c>
       <c r="S35" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T35" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3650,17 +3653,17 @@
         <v>122</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H36" s="8">
         <v>34</v>
@@ -3669,7 +3672,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>20</v>
@@ -3694,7 +3697,7 @@
         <v>155</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T36" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3713,7 +3716,7 @@
         <v>122</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>153</v>
@@ -3721,7 +3724,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="18"/>
       <c r="G37" s="19" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H37" s="8">
         <v>35</v>
@@ -3730,7 +3733,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="20" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="K37" s="21" t="s">
         <v>20</v>
@@ -3743,7 +3746,7 @@
         <v>154</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="P37" s="37" t="s">
         <v>19</v>
@@ -3755,7 +3758,7 @@
         <v>155</v>
       </c>
       <c r="S37" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T37" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3774,7 +3777,7 @@
         <v>122</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D38" s="47" t="s">
         <v>153</v>
@@ -3782,7 +3785,7 @@
       <c r="E38" s="42"/>
       <c r="F38" s="42"/>
       <c r="G38" s="42" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H38" s="40">
         <v>36</v>
@@ -3791,7 +3794,7 @@
         <v>157</v>
       </c>
       <c r="J38" s="42" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K38" s="43" t="s">
         <v>20</v>
@@ -3816,7 +3819,7 @@
         <v>124</v>
       </c>
       <c r="S38" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T38" s="45" t="str">
         <f t="shared" si="0"/>
@@ -3827,7 +3830,7 @@
         <v>RF_08_04_CO</v>
       </c>
       <c r="V38" s="46" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -3838,7 +3841,7 @@
         <v>122</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D39" s="33" t="s">
         <v>160</v>
@@ -3857,7 +3860,7 @@
         <v>156</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>20</v>
@@ -3885,17 +3888,17 @@
         <v>122</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>160</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H40" s="8">
         <v>38</v>
@@ -3904,7 +3907,7 @@
         <v>156</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>20</v>
@@ -3917,7 +3920,7 @@
         <v>33</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P40" s="37" t="s">
         <v>19</v>
@@ -3929,7 +3932,7 @@
         <v>155</v>
       </c>
       <c r="S40" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T40" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3948,10 +3951,10 @@
         <v>122</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -4596,6 +4599,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4610,12 +4619,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">

</xml_diff>